<commit_message>
budget fix from meet 21 Nov
</commit_message>
<xml_diff>
--- a/Budget_Data.xlsx
+++ b/Budget_Data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>Year</t>
   </si>
@@ -52,10 +52,19 @@
     <t>JBBGT</t>
   </si>
   <si>
+    <t>10031</t>
+  </si>
+  <si>
+    <t>UBS/JBBGT/10031/11/2023</t>
+  </si>
+  <si>
+    <t>JBBMT</t>
+  </si>
+  <si>
     <t>10024</t>
   </si>
   <si>
-    <t>UBS/JBBGT/10024/11/2023</t>
+    <t>UBS/JBBMT/10024/11/2023</t>
   </si>
 </sst>
 </file>
@@ -79,7 +88,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -95,6 +104,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE5EEDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -126,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -135,6 +150,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,14 +471,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -508,7 +526,7 @@
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <v>100</v>
       </c>
       <c r="G2" s="3">
@@ -522,9 +540,45 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0</v>
+      </c>
+      <c r="G3" s="4">
+        <v>0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <f>SUM(F3:H3)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="I2">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+      <formula>100</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I3">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>